<commit_message>
Updating Automation Sprint 1 stories
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\qa_auto\wcms-qa-testing-framework\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18825" windowHeight="7605" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18830" windowHeight="7610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Age</t>
   </si>
@@ -88,21 +93,9 @@
     <t>Acute Lymphoblastic Leukemia (ALL)</t>
   </si>
   <si>
-    <t>B Acute Lymphoblastic Leukemia</t>
-  </si>
-  <si>
-    <t>Recurrent Acute Lymphoblastic Leukemia (ALL)</t>
-  </si>
-  <si>
     <t>C3167</t>
   </si>
   <si>
-    <t>C8644%7CC9140%7CC9143</t>
-  </si>
-  <si>
-    <t>C7883%7CC7784</t>
-  </si>
-  <si>
     <t>PSA</t>
   </si>
   <si>
@@ -131,12 +124,111 @@
   </si>
   <si>
     <t>120</t>
+  </si>
+  <si>
+    <t>C142810</t>
+  </si>
+  <si>
+    <t>Recurrent Acute Lymphoblastic Leukemia</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>C122614</t>
+  </si>
+  <si>
+    <t>Infant Acute Lymphoblastic Leukemia</t>
+  </si>
+  <si>
+    <t>Lung Cancer</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>StateCode</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>John F Kennedy Medical Center</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>Antineoplastic Agent</t>
+  </si>
+  <si>
+    <t>DrugId</t>
+  </si>
+  <si>
+    <t>C274</t>
+  </si>
+  <si>
+    <t>Radiation Therapy</t>
+  </si>
+  <si>
+    <t>C15313</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>TreatmentId</t>
+  </si>
+  <si>
+    <t>Physical Therapy</t>
+  </si>
+  <si>
+    <t>C15302</t>
+  </si>
+  <si>
+    <t>C94626</t>
+  </si>
+  <si>
+    <t>Chemoradiotherapy</t>
+  </si>
+  <si>
+    <t>TrialPhase</t>
+  </si>
+  <si>
+    <t>Phase I</t>
+  </si>
+  <si>
+    <t>Phase II</t>
+  </si>
+  <si>
+    <t>Phase III</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,6 +339,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -561,15 +655,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -587,22 +681,33 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>65</v>
-      </c>
-      <c r="C2">
-        <v>20105</v>
+      <c r="B2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3">
-        <v>20105</v>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -613,26 +718,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="18.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.90625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.7265625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="10" style="6" customWidth="1"/>
+    <col min="10" max="13" width="9.1796875" style="2"/>
+    <col min="14" max="14" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1796875" style="2"/>
+    <col min="17" max="17" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -655,13 +766,43 @@
         <v>0</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -681,16 +822,46 @@
         <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -710,42 +881,102 @@
         <v>19</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reviewed with minor updates
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\qa_auto\wcms-qa-testing-framework\test-data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18830" windowHeight="7610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>Age</t>
   </si>
@@ -223,6 +219,51 @@
   </si>
   <si>
     <t>Phase III</t>
+  </si>
+  <si>
+    <t>TrialId</t>
+  </si>
+  <si>
+    <t>E4512</t>
+  </si>
+  <si>
+    <t>A011401,S1207</t>
+  </si>
+  <si>
+    <t>S1207;E4512</t>
+  </si>
+  <si>
+    <t>TrialInvestigator</t>
+  </si>
+  <si>
+    <t>Supriya</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>TrialType</t>
+  </si>
+  <si>
+    <t>Prevention</t>
+  </si>
+  <si>
+    <t>Supportive Care</t>
+  </si>
+  <si>
+    <t>LeadOrganization</t>
+  </si>
+  <si>
+    <t>ECOG-ACRIN Cancer Research Group</t>
+  </si>
+  <si>
+    <t>Alliance for Clinical Trials in Oncology</t>
+  </si>
+  <si>
+    <t>Childrens Oncology Group</t>
+  </si>
+  <si>
+    <t>Lindsay</t>
   </si>
 </sst>
 </file>
@@ -661,12 +702,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -677,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -688,7 +729,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -699,7 +740,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -718,32 +759,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.90625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.7265625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="6" customWidth="1"/>
     <col min="9" max="9" width="10" style="6" customWidth="1"/>
-    <col min="10" max="13" width="9.1796875" style="2"/>
-    <col min="14" max="14" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.1796875" style="2"/>
-    <col min="17" max="17" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.1796875" style="2"/>
+    <col min="10" max="13" width="9.140625" style="2"/>
+    <col min="14" max="14" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="2"/>
+    <col min="18" max="18" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.140625" style="2"/>
+    <col min="21" max="21" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -787,22 +833,34 @@
         <v>48</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="U1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -846,22 +904,34 @@
         <v>49</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="U2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -905,22 +975,34 @@
         <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="U3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -964,19 +1046,31 @@
         <v>49</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor test for valid age searches
Also disable validation of ZIP code search critera on results page.
This should be a search results page test.
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t>Age</t>
   </si>
@@ -128,9 +132,6 @@
     <t>Recurrent Acute Lymphoblastic Leukemia</t>
   </si>
   <si>
-    <t>65</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
@@ -264,6 +265,24 @@
   </si>
   <si>
     <t>Lindsay</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ValidAges</t>
+  </si>
+  <si>
+    <t>InvalidAges</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>chicken</t>
   </si>
 </sst>
 </file>
@@ -696,59 +715,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="9">
+        <v>121</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -818,46 +856,46 @@
         <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="T1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -889,46 +927,46 @@
         <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -960,46 +998,46 @@
         <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="T3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1010,10 +1048,10 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>33</v>
@@ -1031,46 +1069,46 @@
         <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests for Resources for Researchers functionality
* R4R Classes and test data
* Merge R4R test classes.
*  Updated  configuration files.
* Use suite-files structure to make all tests the default.
* Normalize indenting in pom.xml
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\wcms-qa-testing-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="R4R" sheetId="3" r:id="rId3"/>
+    <sheet name="SitewideSearch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
   <si>
     <t>Age</t>
   </si>
@@ -132,6 +134,9 @@
     <t>Recurrent Acute Lymphoblastic Leukemia</t>
   </si>
   <si>
+    <t>65</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
@@ -267,22 +272,55 @@
     <t>Lindsay</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>ValidAges</t>
-  </si>
-  <si>
-    <t>InvalidAges</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>chicken</t>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Terminology</t>
+  </si>
+  <si>
+    <t>Analysis Tools</t>
+  </si>
+  <si>
+    <t>ToolType</t>
+  </si>
+  <si>
+    <t>Datasets &amp; Databases</t>
+  </si>
+  <si>
+    <t>Lab Tools</t>
+  </si>
+  <si>
+    <t>Clinical Research Tools</t>
+  </si>
+  <si>
+    <t>Community Research Tools</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Keyword1</t>
+  </si>
+  <si>
+    <t>Keyword2</t>
+  </si>
+  <si>
+    <t>small cell lung cancer</t>
+  </si>
+  <si>
+    <t>Pancreas</t>
+  </si>
+  <si>
+    <t>pancreatic ductal adenocarcinoma</t>
+  </si>
+  <si>
+    <t>mammography</t>
   </si>
 </sst>
 </file>
@@ -715,78 +753,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9">
-        <v>121</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -799,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -856,46 +875,46 @@
         <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -927,46 +946,46 @@
         <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -998,46 +1017,46 @@
         <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1048,10 +1067,10 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>33</v>
@@ -1069,50 +1088,169 @@
         <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="T4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Tests for Resources for Researchers functionality"
This reverts commit ab2c088e229b18d700fca4a144e4b2355f19f525.
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\wcms-qa-testing-framework\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
-    <sheet name="R4R" sheetId="3" r:id="rId3"/>
-    <sheet name="SitewideSearch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t>Age</t>
   </si>
@@ -134,9 +132,6 @@
     <t>Recurrent Acute Lymphoblastic Leukemia</t>
   </si>
   <si>
-    <t>65</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
@@ -272,55 +267,22 @@
     <t>Lindsay</t>
   </si>
   <si>
-    <t>Cancer</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>Epidemiologic</t>
-  </si>
-  <si>
-    <t>Terminology</t>
-  </si>
-  <si>
-    <t>Analysis Tools</t>
-  </si>
-  <si>
-    <t>ToolType</t>
-  </si>
-  <si>
-    <t>Datasets &amp; Databases</t>
-  </si>
-  <si>
-    <t>Lab Tools</t>
-  </si>
-  <si>
-    <t>Clinical Research Tools</t>
-  </si>
-  <si>
-    <t>Community Research Tools</t>
-  </si>
-  <si>
-    <t>Statistics</t>
-  </si>
-  <si>
-    <t>Keyword1</t>
-  </si>
-  <si>
-    <t>Keyword2</t>
-  </si>
-  <si>
-    <t>small cell lung cancer</t>
-  </si>
-  <si>
-    <t>Pancreas</t>
-  </si>
-  <si>
-    <t>pancreatic ductal adenocarcinoma</t>
-  </si>
-  <si>
-    <t>mammography</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ValidAges</t>
+  </si>
+  <si>
+    <t>InvalidAges</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>chicken</t>
   </si>
 </sst>
 </file>
@@ -753,59 +715,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="9">
+        <v>121</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -875,46 +856,46 @@
         <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="N1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="T1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -946,46 +927,46 @@
         <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -1017,46 +998,46 @@
         <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="T3" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1067,10 +1048,10 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>33</v>
@@ -1088,169 +1069,50 @@
         <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="N4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Merged "wapl-landing" into "pageload-analytics" feature branch (#83)
* Merged latest trunk 
* Removed "Adobe" folder
* Added LandingPage_Test class
* Also added TopicPage_Test class
* Also, also added CthpPage_Test class
* Reworked test classes' Assert() calls for consistency
* Added DoCommonLoadAssertions() method to AnalyticsTestLoadBase
* Moved assertion logic into DoCommonLoadAssertions()
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\qa-automation\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\wcms-qa-testing-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="R4R" sheetId="3" r:id="rId3"/>
+    <sheet name="SitewideSearch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
   <si>
     <t>Age</t>
   </si>
@@ -132,6 +134,9 @@
     <t>Recurrent Acute Lymphoblastic Leukemia</t>
   </si>
   <si>
+    <t>65</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
@@ -267,22 +272,55 @@
     <t>Lindsay</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>ValidAges</t>
-  </si>
-  <si>
-    <t>InvalidAges</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>chicken</t>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Terminology</t>
+  </si>
+  <si>
+    <t>Analysis Tools</t>
+  </si>
+  <si>
+    <t>ToolType</t>
+  </si>
+  <si>
+    <t>Datasets &amp; Databases</t>
+  </si>
+  <si>
+    <t>Lab Tools</t>
+  </si>
+  <si>
+    <t>Clinical Research Tools</t>
+  </si>
+  <si>
+    <t>Community Research Tools</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Keyword1</t>
+  </si>
+  <si>
+    <t>Keyword2</t>
+  </si>
+  <si>
+    <t>small cell lung cancer</t>
+  </si>
+  <si>
+    <t>Pancreas</t>
+  </si>
+  <si>
+    <t>pancreatic ductal adenocarcinoma</t>
+  </si>
+  <si>
+    <t>mammography</t>
   </si>
 </sst>
 </file>
@@ -715,78 +753,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9">
-        <v>121</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -799,7 +818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -856,46 +875,46 @@
         <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -927,46 +946,46 @@
         <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -998,46 +1017,46 @@
         <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
@@ -1048,10 +1067,10 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>33</v>
@@ -1069,50 +1088,169 @@
         <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="T4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding tests for ticket OCEPROJECT-4941 sub-task of OCEPROJECT-4846 (#177)
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\wcms-qa-testing-framework\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nci_workspace\qa_auto\wcms-qa-testing-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{723C3CF2-87E1-42AA-AC41-318ECF00D633}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13785" windowHeight="3360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
     <sheet name="AdvanceSearch" sheetId="2" r:id="rId2"/>
     <sheet name="R4R" sheetId="3" r:id="rId3"/>
-    <sheet name="SitewideSearch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="92">
   <si>
     <t>Age</t>
   </si>
@@ -300,24 +300,6 @@
   </si>
   <si>
     <t>Statistics</t>
-  </si>
-  <si>
-    <t>Keyword1</t>
-  </si>
-  <si>
-    <t>Keyword2</t>
-  </si>
-  <si>
-    <t>small cell lung cancer</t>
-  </si>
-  <si>
-    <t>Pancreas</t>
-  </si>
-  <si>
-    <t>pancreatic ductal adenocarcinoma</t>
-  </si>
-  <si>
-    <t>mammography</t>
   </si>
   <si>
     <t>xTerminologyx</t>
@@ -326,7 +308,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -752,7 +734,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -815,7 +797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1137,7 +1119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1192,7 +1174,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
@@ -1202,55 +1184,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>